<commit_message>
Edits in order to avoid overcorrection
</commit_message>
<xml_diff>
--- a/notebooks/model_extraction/correct_eqs_list_EXCEL.xlsx
+++ b/notebooks/model_extraction/correct_eqs_list_EXCEL.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kovacs.f/Desktop/mira/notebooks/equation extraction development/extraction error check/string mismatch check/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kovacs.f/Desktop/mira/notebooks/model_extraction/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{693F7189-3C59-6545-AAB2-7918B630095A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB17430E-56D1-FB46-8F8E-D2DF85FE8C7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-35780" yWindow="2440" windowWidth="22220" windowHeight="20500" xr2:uid="{30A3DCF3-ADF7-634A-A177-E80CD8B6545B}"/>
+    <workbookView xWindow="-25800" yWindow="0" windowWidth="25800" windowHeight="28800" xr2:uid="{30A3DCF3-ADF7-634A-A177-E80CD8B6545B}"/>
   </bookViews>
   <sheets>
     <sheet name="Munka1" sheetId="1" r:id="rId1"/>
@@ -50,7 +50,137 @@
     <t>BIOMD0000000956</t>
   </si>
   <si>
-    <t>odes = [
+    <t>BIOMD0000000957</t>
+  </si>
+  <si>
+    <t>BIOMD0000000958</t>
+  </si>
+  <si>
+    <t>BIOMD0000000960</t>
+  </si>
+  <si>
+    <t>BIOMD0000000962</t>
+  </si>
+  <si>
+    <t>2024_dec_epi_1_model_A</t>
+  </si>
+  <si>
+    <t>2024_dec_epi_1_model_B</t>
+  </si>
+  <si>
+    <t>2024_dec_epi_1_model_C</t>
+  </si>
+  <si>
+    <t>SAPHIRE</t>
+  </si>
+  <si>
+    <t>BIOMD0000000963</t>
+  </si>
+  <si>
+    <t>BIOMD0000000964</t>
+  </si>
+  <si>
+    <t>BIOMD0000000970</t>
+  </si>
+  <si>
+    <t>BIOMD0000000971</t>
+  </si>
+  <si>
+    <t>BIOMD0000000972</t>
+  </si>
+  <si>
+    <t>BIOMD0000000974</t>
+  </si>
+  <si>
+    <t>BIOMD0000000976</t>
+  </si>
+  <si>
+    <t>BIOMD0000000977</t>
+  </si>
+  <si>
+    <t>BIOMD0000000978</t>
+  </si>
+  <si>
+    <t>BIOMD0000000979</t>
+  </si>
+  <si>
+    <t>BIOMD0000000984</t>
+  </si>
+  <si>
+    <t>BIOMD0000000983</t>
+  </si>
+  <si>
+    <t>BIOMD0000000991</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  [
+    sympy.Eq(S(t).diff(t), Lambda_s - (beta_s + rho_s*(1 - beta_s))*epsilon_s*S(t)*I(t)/N - delta*S(t) + m_s*S_q(t)),
+    sympy.Eq(S_q(t).diff(t), (1 - beta_s)*epsilon_s*rho_s*S(t)*I(t)/N - (m_s + delta)*S_q(t)),
+    sympy.Eq(A(t).diff(t), beta_s*(1 - rho_s)*epsilon_s*S(t)*I(t)/N - (gamma_a + xi_a + delta)*A(t)),
+    sympy.Eq(I(t).diff(t), gamma_a*A(t) - (gamma_i + xi_i + delta)*I(t)),
+    sympy.Eq(I_q(t).diff(t), beta_s*epsilon_s*rho_s*S(t)*I(t)/N + gamma_i*I(t) - (xi_q + delta)*I_q(t)),
+    sympy.Eq(R(t).diff(t), xi_a*A(t) + xi_i*I(t) + xi_q*I_q(t) - delta*R(t))
+]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  [
+    sympy.Eq(S(t).diff(t), -(1 - epsilon)*beta*S(t)*I(t)/N),
+    sympy.Eq(E(t).diff(t), (1 - epsilon)*beta*S(t)*I(t)/N - sigma*E(t)),
+    sympy.Eq(I(t).diff(t), sigma*E(t) - gamma*I(t)),
+    sympy.Eq(R(t).diff(t), gamma*I(t))
+]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  [
+    sympy.Eq(S(t).diff(t), -beta(t)*S(t)/N*I(t) + omega*R(t)),
+    sympy.Eq(E(t).diff(t), beta(t)*S(t)/N*I(t) - sigma*E(t)),
+    sympy.Eq(I(t).diff(t), sigma*E(t) - gamma*I(t)),
+    sympy.Eq(R(t).diff(t), gamma*I(t) - omega*R(t))
+]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  [
+    sympy.Eq(S_c(t).diff(t), m(t)*S_u(t) - (1 - m(t))*S_c(t)),
+    sympy.Eq(S_u(t).diff(t), (1 - m(t))*S_c(t) - m(t)*S_u(t) - beta*(n*I_r(t) + I_u(t))*S_u(t) + theta*(1 - lambda_)*Q(t)),
+    sympy.Eq(E(t).diff(t), (1 - sigma)*beta*(n*I_r(t) + I_u(t))*S_u(t) - mu*E(t)),
+    sympy.Eq(I_r(t).diff(t), mu*f*E(t) + theta*lambda_*Q(t) - eta_r*I_r(t)),
+    sympy.Eq(I_u(t).diff(t), mu*(1 - f)*E(t) - eta_u*I_u(t)),
+    sympy.Eq(R(t).diff(t), eta_r*q*I_r(t) + eta_u*I_u(t)),
+    sympy.Eq(Q(t).diff(t), sigma*beta*(n*I_r(t) + I_u(t))*S_u(t) - theta*Q(t))
+]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  [
+    sympy.Eq(S(t).diff(t), -beta*S(t)/N*I(t)),
+    sympy.Eq(E(t).diff(t), beta*S(t)/N*I(t) - omega*E(t)),
+    sympy.Eq(I(t).diff(t), omega*E(t) - gamma*I(t)),
+    sympy.Eq(R(t).diff(t), gamma*I(t))
+]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  [
+    sympy.Eq(S(t).diff(t), -beta_c*(alpha*A(t) + I(t))*S(t)/(N_h - I_D(t))),
+    sympy.Eq(E(t).diff(t), beta_c*(alpha*A(t) + I(t))*S(t)/(N_h - I_D(t)) - sigma*E(t)),
+    sympy.Eq(A(t).diff(t), nu*sigma*E(t) - (theta + gamma_a)*A(t)),
+    sympy.Eq(I(t).diff(t), (1 - nu)*sigma*E(t) - (psi + gamma_O + d_O)*I(t)),
+    sympy.Eq(I_D(t).diff(t), theta*A(t) + psi*I(t) - (gamma_i + d_D)*I_D(t)),
+    sympy.Eq(R(t).diff(t), gamma_i*I_D(t) + gamma_a*A(t) + gamma_O*I(t))
+]</t>
+  </si>
+  <si>
+    <t>[
+    sympy.Eq(S(t).diff(t), - S(t) * (alpha * I(t) + beta * D(t) + gamma * A(t) + delta * R(t))),
+    sympy.Eq(I(t).diff(t), S(t) * (alpha * I(t) + beta * D(t) + gamma * A(t) + delta * R(t)) - (epsilon + zeta + lambda_) * I(t)),
+    sympy.Eq(D(t).diff(t), epsilon * I(t) - (eta + rho) * D(t)),
+    sympy.Eq(A(t).diff(t), zeta * I(t) - (theta + mu + kappa) * A(t)),
+    sympy.Eq(R(t).diff(t), eta * D(t) + theta * A(t) - (nu + xi) * R(t)),
+    sympy.Eq(T(t).diff(t), mu * A(t) + nu * R(t) - (sigma + tau) * T(t)),
+    sympy.Eq(H(t).diff(t), lambda_ * I(t) + rho * D(t) + kappa * A(t) + xi * R(t) + sigma * T(t)),
+    sympy.Eq(E(t).diff(t), tau * T(t))
+]</t>
+  </si>
+  <si>
+    <t>[
     sympy.Eq(S(t).diff(t), - beta * S(t) * I(t) / N),
     sympy.Eq(E(t).diff(t), beta * S(t) * I(t) / N - alpha * E(t)),
     sympy.Eq(I(t).diff(t), alpha * E(t) - gamma * I(t)),
@@ -58,13 +188,7 @@
 ]</t>
   </si>
   <si>
-    <t>BIOMD0000000957</t>
-  </si>
-  <si>
-    <t>BIOMD0000000958</t>
-  </si>
-  <si>
-    <t>odes = [
+    <t>[
     sympy.Eq(S(t).diff(t), - beta * S(t) * I(t)),
     sympy.Eq(E(t).diff(t), beta * S(t) * I(t) - epsilon * E(t)),
     sympy.Eq(I(t).diff(t), epsilon * E(t) - (rho + mu) * I(t)),
@@ -72,7 +196,7 @@
 ]</t>
   </si>
   <si>
-    <t>odes = [
+    <t>[
     sympy.Eq(S(t).diff(t), -beta * I(t) / N * S(t) - l * beta * H(t) / N * S(t) - beta_prime * P(t) / N * S(t)),
     sympy.Eq(E(t).diff(t), beta * I(t) / N * S(t) + l * beta * H(t) / N * S(t) + beta_prime * P(t)/N * S(t) - kappa * E(t)),
     sympy.Eq(I(t).diff(t), kappa * rho1 * E(t) - (gamma_alpha + gamma_i) * I(t) - delta_i * I(t)),
@@ -84,10 +208,7 @@
 ]</t>
   </si>
   <si>
-    <t>BIOMD0000000960</t>
-  </si>
-  <si>
-    <t>odes = [
+    <t>[
     sympy.Eq(S(t).diff(t), - S(t) * beta * (I(t) + l_a * A(t) + l * H(t)) / N),
     sympy.Eq(E(t).diff(t), S(t) * beta * (I(t) + l_a * A(t) + l * H(t)) / N - kappa * E(t)),
     sympy.Eq(I(t).diff(t), kappa * rho * E(t) - (gamma_a + gamma_I + delta_I) * I(t)),
@@ -98,10 +219,7 @@
 ]</t>
   </si>
   <si>
-    <t>BIOMD0000000962</t>
-  </si>
-  <si>
-    <t>odes = [
+    <t>[
     sympy.Eq(S(t).diff(t), -a * U(t) * S(t) / N),
     sympy.Eq(U(t).diff(t), a * U(t) * S(t) / N - gamma1 * U(t)),
     sympy.Eq(Q(t).diff(t), gamma1 * U(t) - (gamma2 + (1 - gamma2) * sigma) * Q(t)),
@@ -109,10 +227,7 @@
 ]</t>
   </si>
   <si>
-    <t>2024_dec_epi_1_model_A</t>
-  </si>
-  <si>
-    <t>odes = [
+    <t>[
     sympy.Eq(s1(t).diff(t), pi_h * (1 - rho) - nu * lambda_h * s1(t) - mu_h * s1(t)),
     sympy.Eq(s_h(t).diff(t), mu_h * rho - lambda_h * s_h(t) - mu_h * s_h(t)),
     sympy.Eq(e_h(t).diff(t), (nu * s1(t) + s_h(t)) * lambda_h - (sigma + mu_h) * e_h(t)),
@@ -128,10 +243,7 @@
 ]</t>
   </si>
   <si>
-    <t>2024_dec_epi_1_model_B</t>
-  </si>
-  <si>
-    <t>odes = [
+    <t>[
     sympy.Eq(sh(t).diff(t), beta_h - (beta_1 * ir(t) + beta_2 * ih(t)) * sh(t) / N_h - mu_h * sh(t) + phi * qh(t)),
     sympy.Eq(eh(t).diff(t), (beta_1 * ir(t) + beta_2 * ih(t)) * sh(t) / N_h - (alpha_1 + alpha_2 + mu_h) * eh(t)),
     sympy.Eq(ih(t).diff(t), alpha_1 * eh(t) - (mu_h + delta_h + gamma) * ih(t)),
@@ -143,7 +255,7 @@
 ]</t>
   </si>
   <si>
-    <t>odes = [
+    <t>[
     sympy.Eq(s_m(t).diff(t), - lambda_m * s_m(t)),
     sympy.Eq(e_m(t).diff(t), lambda_m * s_m(t) - alpha_m * e_m(t)),
     sympy.Eq(i_m(t).diff(t), alpha_m * e_m(t) - tau_m * i_m(t)),
@@ -155,13 +267,7 @@
 ]</t>
   </si>
   <si>
-    <t>2024_dec_epi_1_model_C</t>
-  </si>
-  <si>
-    <t>SAPHIRE</t>
-  </si>
-  <si>
-    <t>odes = [
+    <t>[
     sympy.Eq(S(t).diff(t), n - b * (alpha * P(t) + alpha * A(t) + l) / N * S(t) - n * S(t) / N),
     sympy.Eq(E(t).diff(t), b * (alpha * P(t) + alpha * A(t) + l) / N * S(t) - E(t) / De - n * E(t) / N),
     sympy.Eq(P(t).diff(t), E(t) / De - P(t) / Dp - n * P(t)/N),
@@ -172,73 +278,14 @@
 ]</t>
   </si>
   <si>
-    <t>odes = [
-    sympy.Eq(S(t).diff(t), - S(t) * (alpha * I(t) + beta * D(t) + gamma * A(t) + delta * R(t))),
-    sympy.Eq(I(t).diff(t), S(t) * (alpha * I(t) + beta * D(t) + gamma * A(t) + delta * R(t)) - (epsilon + zeta + lambda_) * I(t)),
-    sympy.Eq(D(t).diff(t), epsilon * I(t) - (eta + rho) * D(t)),
-    sympy.Eq(A(t).diff(t), zeta * I(t) - (theta + mu + kappa) * A(t)),
-    sympy.Eq(R(t).diff(t), eta * D(t) + theta * A(t) - (nu + xi) * R(t)),
-    sympy.Eq(T(t).diff(t), mu * A(t) + nu * R(t) - (sigma + tau) * T(t)),
-    sympy.Eq(H(t).diff(t), lambda_ * I(t) + rho * D(t) + kappa * A(t) + xi * R(t) + sigma * T(t)),
-    sympy.Eq(E(t).diff(t), tau * T(t))
-]</t>
-  </si>
-  <si>
-    <t>BIOMD0000000963</t>
-  </si>
-  <si>
-    <t>BIOMD0000000964</t>
-  </si>
-  <si>
-    <t>BIOMD0000000970</t>
-  </si>
-  <si>
-    <t>BIOMD0000000971</t>
-  </si>
-  <si>
-    <t>BIOMD0000000972</t>
-  </si>
-  <si>
-    <t>BIOMD0000000974</t>
-  </si>
-  <si>
-    <t>BIOMD0000000976</t>
-  </si>
-  <si>
-    <t>BIOMD0000000977</t>
-  </si>
-  <si>
-    <t>odes = [
-    sympy.Eq(S(t).diff(t), -tau(t)*S(t)*(I_1(t) + I_2(t))),
-    sympy.Eq(I_1(t).diff(t), alpha*tau(t)*S(t)*(I_1(t) + I_2(t)) - gamma_1*I_1(t)),
-    sympy.Eq(I_2(t).diff(t), (1 - alpha)*tau(t)*S(t)*(I_1(t) + I_2(t)) - (gamma_2 + mu)*I_2(t)),
-    sympy.Eq(R(t).diff(t), gamma_1*I_1(t) + gamma_2*I_2(t))
-]</t>
-  </si>
-  <si>
-    <t>BIOMD0000000978</t>
-  </si>
-  <si>
-    <t>BIOMD0000000979</t>
-  </si>
-  <si>
-    <t>BIOMD0000000984</t>
-  </si>
-  <si>
-    <t>BIOMD0000000983</t>
-  </si>
-  <si>
-    <t>BIOMD0000000991</t>
-  </si>
-  <si>
-    <t>odes = [
+    <t>[
     sympy.Eq(S(t).diff(t), -beta * S(t) * I(t) / (1 + alpha*R(t))),
     sympy.Eq(I(t).diff(t), beta * S(t) * I(t) / (1 + alpha*R(t)) - gamma*I(t)),
     sympy.Eq(R(t).diff(t), gamma*I(t))
 ]</t>
   </si>
   <si>
-    <t>odes = [
+    <t>[
     sympy.Eq(S(t).diff(t), b - (beta_1*S(t)*P(t))/(1+alpha_1*P(t)) - (beta_2*S(t)*(I_A(t)+I_S(t)))/(1+alpha_2*(I_A(t)+I_S(t))) + psi*E(t) - mu*S(t)),
     sympy.Eq(E(t).diff(t), (beta_1*S(t)*P(t))/(1+alpha_1*P(t)) + (beta_2*S(t)*(I_A(t)+I_S(t)))/(1+alpha_2*(I_A(t)+I_S(t))) - psi*E(t) - mu*E(t) - omega*E(t)),
     sympy.Eq(I_A(t).diff(t), (1-delta)*omega*E(t) - (mu+sigma)*I_A(t) - gamma_A*I_A(t)),
@@ -248,7 +295,7 @@
 ]</t>
   </si>
   <si>
-    <t>odes = [
+    <t>[
     sympy.Eq(S(t).diff(t), -r_1*beta_1*I(t)*S(t)/N - r_2*beta_2*E(t)*S(t)/N),
     sympy.Eq(E(t).diff(t), r_1*beta*I(t)*S(t)/N - alpha*E(t) + r_2*beta_2*E(t)*S(t)/N),
     sympy.Eq(I(t).diff(t), alpha*E(t) - gamma*I(t)),
@@ -256,7 +303,7 @@
 ]</t>
   </si>
   <si>
-    <t>odes = [
+    <t>[
     sympy.Eq(S(t).diff(t), -(beta*c + c*q*(1 - beta))*S(t)*(I(t) + theta*A(t)) + lambda_*S_q(t)),
     sympy.Eq(E(t).diff(t), beta*c*(1 - q)*S(t)*(I(t) + theta*A(t)) - sigma*E(t)),
     sympy.Eq(I(t).diff(t), sigma*rho*E(t) - (delta_I + alpha + gamma_I)*I(t)),
@@ -268,7 +315,7 @@
 ]</t>
   </si>
   <si>
-    <t>odes = [
+    <t>[
     sympy.Eq(S(t).diff(t), -(beta*c(t) + c(t)*q*(1 - beta))*S(t)*(I(t) + theta*A(t)) + lambda_*S_q(t)),
     sympy.Eq(E(t).diff(t), beta*c(t)*(1 - q)*S(t)*(I(t) + theta*A(t)) - sigma*E(t)),
     sympy.Eq(I(t).diff(t), sigma*rho*E(t) - (delta_I(t) + alpha + gamma_I)*I(t)),
@@ -280,7 +327,7 @@
 ]</t>
   </si>
   <si>
-    <t>odes = [
+    <t>[
     sympy.Eq(S(t).diff(t), Lambda - mu*S(t) - beta*S(t)*I(t)/N),
     sympy.Eq(E(t).diff(t), beta*S(t)*I(t)/N - (mu + epsilon)*E(t)),
     sympy.Eq(I(t).diff(t), epsilon*E(t) - (gamma + mu + alpha)*I(t)),
@@ -288,58 +335,11 @@
 ]</t>
   </si>
   <si>
-    <t>odes = [
-    sympy.Eq(S(t).diff(t), Lambda_s - (beta_s + rho_s*(1 - beta_s))*epsilon_s*S(t)*I(t)/N - delta*S(t) + m_s*S_q(t)),
-    sympy.Eq(S_q(t).diff(t), (1 - beta_s)*epsilon_s*rho_s*S(t)*I(t)/N - (m_s + delta)*S_q(t)),
-    sympy.Eq(A(t).diff(t), beta_s*(1 - rho_s)*epsilon_s*S(t)*I(t)/N - (gamma_a + xi_a + delta)*A(t)),
-    sympy.Eq(I(t).diff(t), gamma_a*A(t) - (gamma_i + xi_i + delta)*I(t)),
-    sympy.Eq(I_q(t).diff(t), beta_s*epsilon_s*rho_s*S(t)*I(t)/N + gamma_i*I(t) - (xi_q + delta)*I_q(t)),
-    sympy.Eq(R(t).diff(t), xi_a*A(t) + xi_i*I(t) + xi_q*I_q(t) - delta*R(t))
-]</t>
-  </si>
-  <si>
-    <t>odes = [
-    sympy.Eq(S(t).diff(t), -(1 - epsilon)*beta*S(t)*I(t)/N),
-    sympy.Eq(E(t).diff(t), (1 - epsilon)*beta*S(t)*I(t)/N - sigma*E(t)),
-    sympy.Eq(I(t).diff(t), sigma*E(t) - gamma*I(t)),
-    sympy.Eq(R(t).diff(t), gamma*I(t))
-]</t>
-  </si>
-  <si>
-    <t>odes = [
-    sympy.Eq(S_c(t).diff(t), m(t)*S_u(t) - (1 - m(t))*S_c(t)),
-    sympy.Eq(S_u(t).diff(t), (1 - m(t))*S_c(t) - m(t)*S_u(t) - beta*(n*I_r(t) + I_u(t))*S_u(t) + theta*(1 - lambda_)*Q(t)),
-    sympy.Eq(E(t).diff(t), (1 - sigma)*beta*(n*I_r(t) + I_u(t))*S_u(t) - mu*E(t)),
-    sympy.Eq(I_r(t).diff(t), mu*f*E(t) + theta*lambda_*Q(t) - eta_r*I_r(t)),
-    sympy.Eq(I_u(t).diff(t), mu*(1 - f)*E(t) - eta_u*I_u(t)),
-    sympy.Eq(R(t).diff(t), eta_r*q*I_r(t) + eta_u*I_u(t)),
-    sympy.Eq(Q(t).diff(t), sigma*beta*(n*I_r(t) + I_u(t))*S_u(t) - theta*Q(t))
-]</t>
-  </si>
-  <si>
-    <t>odes = [
-    sympy.Eq(S(t).diff(t), -beta*S(t)/N*I(t)),
-    sympy.Eq(E(t).diff(t), beta*S(t)/N*I(t) - omega*E(t)),
-    sympy.Eq(I(t).diff(t), omega*E(t) - gamma*I(t)),
-    sympy.Eq(R(t).diff(t), gamma*I(t))
-]</t>
-  </si>
-  <si>
-    <t>odes = [
-    sympy.Eq(S(t).diff(t), -beta_c*(alpha*A(t) + I(t))*S(t)/(N_h - I_D(t))),
-    sympy.Eq(E(t).diff(t), beta_c*(alpha*A(t) + I(t))*S(t)/(N_h - I_D(t)) - sigma*E(t)),
-    sympy.Eq(A(t).diff(t), nu*sigma*E(t) - (theta + gamma_a)*A(t)),
-    sympy.Eq(I(t).diff(t), (1 - nu)*sigma*E(t) - (psi + gamma_O + d_O)*I(t)),
-    sympy.Eq(I_D(t).diff(t), theta*A(t) + psi*I(t) - (gamma_i + d_D)*I_D(t)),
-    sympy.Eq(R(t).diff(t), gamma_i*I_D(t) + gamma_a*A(t) + gamma_O*I(t))
-]</t>
-  </si>
-  <si>
-    <t>odes = [
-    sympy.Eq(S(t).diff(t), -beta(t)*S(t)/N*I(t) + omega*R(t)),
-    sympy.Eq(E(t).diff(t), beta(t)*S(t)/N*I(t) - sigma*E(t)),
-    sympy.Eq(I(t).diff(t), sigma*E(t) - gamma*I(t)),
-    sympy.Eq(R(t).diff(t), gamma*I(t) - omega*R(t))
+    <t>[
+    sympy.Eq(S(t).diff(t), -tau(t)*S(t)*(I_1(t) + I_2(t))),
+    sympy.Eq(I_1(t).diff(t), alpha*tau(t)*S(t)*(I_1(t) + I_2(t)) - gamma_1*I_1(t)),
+    sympy.Eq(I_2(t).diff(t), (1 - alpha)*tau(t)*S(t)*(I_1(t) + I_2(t)) - (gamma_2 + mu)*I_2(t)),
+    sympy.Eq(R(t).diff(t), gamma_1*I_1(t) + gamma_2*I_2(t))
 ]</t>
   </si>
 </sst>
@@ -391,15 +391,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -738,208 +735,208 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{585F8C20-F92E-4147-81E7-1FDA03FC9F94}">
   <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="68.5" style="2" customWidth="1"/>
-    <col min="3" max="3" width="83.1640625" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="10.83203125" style="2"/>
+    <col min="1" max="1" width="22.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="68.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="83.1640625" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="221" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="102" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="102" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="255" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="153" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="102" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="255" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="238" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="170" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="170" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="85" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="221" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="119" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="187" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="204" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="102" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="119" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="204" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="102" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="102" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" ht="102" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="102" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="255" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="153" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="102" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="255" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="238" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="170" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="170" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="85" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
+      <c r="B21" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="170" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="102" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="221" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="119" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
+      <c r="B23" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="136" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="187" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="204" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="102" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="119" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B18" s="3" t="s">
+      <c r="B24" s="1" t="s">
         <v>30</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="204" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="102" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="102" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="170" x14ac:dyDescent="0.2">
-      <c r="A22" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="102" x14ac:dyDescent="0.2">
-      <c r="A23" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" ht="136" x14ac:dyDescent="0.2">
-      <c r="A24" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>